<commit_message>
Remove the detection point column as that will be put into another spreadsheet in GHT/
</commit_message>
<xml_diff>
--- a/DicomSubsampling/reference_info.xlsx
+++ b/DicomSubsampling/reference_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 1\ESC499 - Thesis\Undergraduate_Thesis_Scripts\DicomSubsampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFFC0AD-834E-493F-B637-C02B85E84E3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B446D57F-1DC5-4B41-9080-976436089B9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -31,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>x is left to right, y is up to down, z is into the page</t>
-  </si>
-  <si>
-    <t>Detection Point</t>
   </si>
   <si>
     <t>x1</t>
@@ -440,21 +437,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.6328125" customWidth="1"/>
     <col min="2" max="7" width="6.6328125" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" customWidth="1"/>
-    <col min="9" max="9" width="54.90625" customWidth="1"/>
+    <col min="8" max="8" width="54.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -465,38 +461,34 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>6268647</v>
       </c>
@@ -518,9 +510,8 @@
       <c r="G3" s="4">
         <v>28</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>6729799</v>
       </c>
@@ -542,9 +533,8 @@
       <c r="G4" s="4">
         <v>28</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>7796800</v>
       </c>
@@ -566,12 +556,11 @@
       <c r="G5" s="4">
         <v>25</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>8214092</v>
       </c>
@@ -593,9 +582,8 @@
       <c r="G6" s="4">
         <v>29</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>8285119</v>
       </c>
@@ -617,9 +605,8 @@
       <c r="G7" s="4">
         <v>27</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>8476267</v>
       </c>
@@ -641,9 +628,8 @@
       <c r="G8" s="4">
         <v>25</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8512802</v>
       </c>
@@ -665,9 +651,8 @@
       <c r="G9" s="4">
         <v>29</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>8931305</v>
       </c>
@@ -689,9 +674,8 @@
       <c r="G10" s="4">
         <v>37</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>8949024</v>
       </c>
@@ -713,12 +697,11 @@
       <c r="G11" s="4">
         <v>29</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>9049401</v>
       </c>
@@ -740,9 +723,8 @@
       <c r="G12" s="4">
         <v>32</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -750,9 +732,8 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -760,9 +741,8 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -770,9 +750,8 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -780,9 +759,8 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -790,9 +768,8 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -800,9 +777,8 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -810,9 +786,8 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -820,9 +795,8 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -830,9 +804,8 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -840,9 +813,8 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -850,9 +822,8 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -860,9 +831,8 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -870,9 +840,8 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -880,9 +849,8 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -890,9 +858,8 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -900,9 +867,8 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -910,9 +876,8 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -920,9 +885,8 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -930,9 +894,8 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -940,9 +903,8 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -950,9 +912,8 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -960,9 +921,8 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -970,9 +930,8 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -980,9 +939,8 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -990,9 +948,8 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1000,14 +957,13 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H12">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified error in ac_num
</commit_message>
<xml_diff>
--- a/DicomSubsampling/reference_info.xlsx
+++ b/DicomSubsampling/reference_info.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\DicomSubsampling\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC55C45-9C78-4A2D-AF39-1DC899AE9AFB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12105"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Boundaries" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,25 +423,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="7" width="6.6328125" customWidth="1"/>
-    <col min="8" max="8" width="54.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -677,7 +671,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>8949024</v>
+        <v>8649024</v>
       </c>
       <c r="B11" s="3">
         <v>23</v>
@@ -959,7 +953,7 @@
       <c r="G38" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H12">
+  <sortState ref="A3:H12">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated references slightly for better accuracy
</commit_message>
<xml_diff>
--- a/DicomSubsampling/reference_info.xlsx
+++ b/DicomSubsampling/reference_info.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>x1</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>Accession Num</t>
-  </si>
-  <si>
-    <t>Smaller by around 10-20%</t>
-  </si>
-  <si>
-    <t>Ideal</t>
   </si>
   <si>
     <t>x is top to bottom, y is left to right, z is out of the page</t>
@@ -109,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -117,6 +111,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +429,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +441,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -499,10 +494,10 @@
         <v>60</v>
       </c>
       <c r="F3" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -510,10 +505,10 @@
         <v>6729799</v>
       </c>
       <c r="B4" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3">
         <v>26</v>
@@ -545,13 +540,10 @@
         <v>66</v>
       </c>
       <c r="F5" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -559,22 +551,22 @@
         <v>8214092</v>
       </c>
       <c r="B6" s="3">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44</v>
+      </c>
+      <c r="E6" s="3">
+        <v>68</v>
+      </c>
+      <c r="F6" s="3">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
-        <v>47</v>
-      </c>
-      <c r="D6" s="3">
-        <v>46</v>
-      </c>
-      <c r="E6" s="3">
-        <v>70</v>
-      </c>
-      <c r="F6" s="3">
-        <v>11</v>
-      </c>
       <c r="G6" s="3">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -582,19 +574,19 @@
         <v>8285119</v>
       </c>
       <c r="B7" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F7" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="3">
         <v>27</v>
@@ -605,22 +597,22 @@
         <v>8476267</v>
       </c>
       <c r="B8" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D8" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E8" s="3">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F8" s="3">
         <v>9</v>
       </c>
       <c r="G8" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -628,71 +620,68 @@
         <v>8512802</v>
       </c>
       <c r="B9" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F9" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>8931305</v>
+        <v>8649024</v>
       </c>
       <c r="B10" s="3">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3">
-        <v>56</v>
+        <v>22</v>
+      </c>
+      <c r="C10" s="5">
+        <v>59</v>
       </c>
       <c r="D10" s="3">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F10" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>8649024</v>
+        <v>8931305</v>
       </c>
       <c r="B11" s="3">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="F11" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G11" s="3">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -706,10 +695,10 @@
         <v>48</v>
       </c>
       <c r="D12" s="3">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="3">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" s="3">
         <v>13</v>

</xml_diff>